<commit_message>
Actualizacion ejecuciones de casos de pruebas
</commit_message>
<xml_diff>
--- a/Producto/Web/Casos de prueba/17.xlsx
+++ b/Producto/Web/Casos de prueba/17.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="315" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="6810" yWindow="315" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DatosGenerales" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Pasos" sheetId="2" r:id="rId3"/>
     <sheet name="Control de cambios" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -79,21 +79,6 @@
     <t>Existen playas en la ciudad de Córdoba</t>
   </si>
   <si>
-    <t>Escribo "cordoba" en donde se debe ingresar la ciudad a buscar.</t>
-  </si>
-  <si>
-    <t>Se muestra el autocomplete con las opciones de las ciudad que se corresponden con la cadena "cordoba".</t>
-  </si>
-  <si>
-    <t>Selecciono "Córdoba, Argentina" en la lista de ciudad del autocomplete y presiono BUSCAR</t>
-  </si>
-  <si>
-    <t>Me redirige a la pagina "BusquedaPlayas.aspx" y se muestra en el mapa la ciudad de Córdoba y las playas de esa ciudad.</t>
-  </si>
-  <si>
-    <t>ingreso al sitio web.</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
@@ -109,27 +94,12 @@
     <t>Esta iniciada la sesion de un usuario con rol administrador</t>
   </si>
   <si>
-    <t>Ingreso a la opcion Estadisticas</t>
-  </si>
-  <si>
-    <t>Presiono el boton "Nueva"</t>
-  </si>
-  <si>
     <t>Se despliegan 2 opciones, "Historica" y "Tiempo Real"</t>
   </si>
   <si>
-    <t>Presiono el boton "Historica"</t>
-  </si>
-  <si>
     <t>Se muestra un panel para buscar estadisticas historicas</t>
   </si>
   <si>
-    <t>Ingreso Estaddistica: "Consulta", Por: "Playa",Desde 01/01/2014, Hasta 01/03/2015</t>
-  </si>
-  <si>
-    <t>Presiono el boton "Buscar"</t>
-  </si>
-  <si>
     <t>Se despliega el panel de estadisticas, con los filtros y las opciones del grafico</t>
   </si>
   <si>
@@ -137,13 +107,46 @@
   </si>
   <si>
     <t>25</t>
+  </si>
+  <si>
+    <t>Ingresar al sitio web.</t>
+  </si>
+  <si>
+    <t>Ingresar a la opcion Estadisticas</t>
+  </si>
+  <si>
+    <t>Escribir &lt;Ciudad1&gt; en donde se debe ingresar la ciudad a buscar.</t>
+  </si>
+  <si>
+    <t>Seleccionar &lt;Ciudad1&gt; en la lista de ciudad del autocomplete y presiono BUSCAR</t>
+  </si>
+  <si>
+    <t>Presionar el boton "Nueva"</t>
+  </si>
+  <si>
+    <t>Presionar el boton "Historica"</t>
+  </si>
+  <si>
+    <t>Presionar el boton "Buscar"</t>
+  </si>
+  <si>
+    <t>Ingresar Estaddistica: "Consulta", Por: "Playa",Desde 01/01/2014, Hasta 01/03/2015</t>
+  </si>
+  <si>
+    <t>Presionar el boton Buscar</t>
+  </si>
+  <si>
+    <t>Se muestra el autocomplete con las opciones de las ciudad que se corresponden con &lt;Ciudad1&gt;</t>
+  </si>
+  <si>
+    <t>Se abre un panel para configurar las estadisticas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -292,22 +295,60 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF548DD4"/>
+        <color theme="3" tint="0.39997558519241921"/>
       </left>
       <right style="medium">
         <color rgb="FF548DD4"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color theme="3" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3" tint="0.39997558519241921"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF548DD4"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <right style="medium">
+        <color rgb="FF548DD4"/>
+      </right>
+      <top style="medium">
+        <color theme="3" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF548DD4"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="0.39997558519241921"/>
+      </right>
+      <top style="medium">
+        <color theme="3" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3" tint="0.39997558519241921"/>
+      </right>
+      <top style="medium">
+        <color theme="3" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3" tint="0.39997558519241921"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -315,7 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -347,12 +388,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -443,6 +488,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -477,6 +523,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -652,44 +699,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="26.25" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="26.25" thickBot="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="32.25" thickBot="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -697,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.5" thickBot="1">
+    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -706,15 +753,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.5" thickBot="1">
+    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16.5" thickBot="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -732,20 +779,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1">
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -756,7 +803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -764,20 +811,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -789,19 +836,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="B2:C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.140625" customWidth="1"/>
     <col min="3" max="3" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -815,92 +864,100 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="39" thickBot="1">
+    <row r="4" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="39" thickBot="1">
+    <row r="5" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="26.25" thickBot="1">
-      <c r="A6" s="7">
+        <v>33</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="25.5">
-      <c r="A7" s="7">
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="25.5">
-      <c r="A8" s="12">
+      <c r="B8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="25.5">
-      <c r="A9" s="12">
+      <c r="B9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="16"/>
+    </row>
+    <row r="10" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="12"/>
+      <c r="C10" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -911,14 +968,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -926,7 +983,7 @@
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -943,7 +1000,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="38.25">
+    <row r="2" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
@@ -954,7 +1011,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>18</v>

</xml_diff>